<commit_message>
exercice postman, conception & readme
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8316FB65-596E-4168-9EB9-3EA70BC5C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3BBE07-4B90-46E5-8862-339AD7A9AF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
   <si>
     <t>Tâches</t>
   </si>
@@ -382,12 +382,27 @@
   <si>
     <t>Correction Analyse</t>
   </si>
+  <si>
+    <t>Exercice Postman</t>
+  </si>
+  <si>
+    <t>Diagramme de sequence interaction sur EA (sport)</t>
+  </si>
+  <si>
+    <t>Structure de fichier du serveur</t>
+  </si>
+  <si>
+    <t>Structure de fichier du client</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +486,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -533,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -841,31 +863,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -880,19 +926,96 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -900,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -934,9 +1057,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -946,32 +1066,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -986,19 +1082,73 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1031,91 +1181,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1126,10 +1288,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FFFFFFCC"/>
-      <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1435,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1446,73 +1608,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46" t="str">
+      <c r="B3" s="55" t="str">
         <f>'Journal de travail'!B3</f>
         <v xml:space="preserve">Simon Gendre </v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="46">
+      <c r="P3" s="55">
         <v>300633</v>
       </c>
-      <c r="Q3" s="48"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="46" t="str">
+      <c r="B4" s="55" t="str">
         <f>'Journal de travail'!B4</f>
         <v>Semaphor</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="48"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="57"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1522,32 +1684,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="49" t="s">
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="49" t="s">
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="49" t="s">
+      <c r="M7" s="59"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="51"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1604,659 +1766,667 @@
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="42" t="s">
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="61"/>
+      <c r="I9" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="35"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="36"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="61"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="61"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="36"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="61"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="36"/>
     </row>
     <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="61"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="36"/>
     </row>
     <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="61"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="36"/>
     </row>
     <row r="14" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="59" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="61"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="36"/>
     </row>
     <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="61"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="36"/>
     </row>
     <row r="16" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="59" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="F16" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="61"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="61"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="59" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="60"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="61"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="36"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="61"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="36"/>
     </row>
     <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="61"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="36"/>
     </row>
     <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="66" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="61"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="36"/>
     </row>
     <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="61"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="61"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="36"/>
     </row>
     <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="60" t="s">
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="61"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="35"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="36"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="61"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="36"/>
     </row>
     <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="61"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" s="35"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="36"/>
     </row>
     <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="61"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="36"/>
     </row>
     <row r="26" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="61"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="36"/>
     </row>
     <row r="27" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="61"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="36"/>
     </row>
     <row r="28" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="61"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="36"/>
     </row>
     <row r="29" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="61"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="35"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="36"/>
     </row>
     <row r="30" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="61"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="36"/>
     </row>
     <row r="31" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="61"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="36"/>
     </row>
     <row r="32" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="61"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="36"/>
     </row>
     <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="70"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="61"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="36"/>
     </row>
     <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="59"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="61"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="36"/>
     </row>
     <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="59"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="59"/>
-      <c r="P35" s="60"/>
-      <c r="Q35" s="68"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="34"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="43"/>
     </row>
     <row r="36" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="71"/>
-      <c r="P36" s="60"/>
-      <c r="Q36" s="61"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="36"/>
     </row>
     <row r="37" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="61"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="36"/>
+      <c r="O37" s="34"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="36"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="74"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="48"/>
+      <c r="Q38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
@@ -2288,25 +2458,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2328,262 +2498,326 @@
       <c r="C4" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="71">
         <v>45320</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26">
+      <c r="A9" s="70">
         <v>45321</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="82">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="74">
         <v>45327</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="83">
         <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
-        <v>45327</v>
-      </c>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="75"/>
+      <c r="B11" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="84">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
-        <v>45327</v>
-      </c>
-      <c r="B12" s="38" t="s">
+      <c r="A12" s="75"/>
+      <c r="B12" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="84">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
-        <v>45327</v>
-      </c>
-      <c r="B13" s="38" t="s">
+      <c r="A13" s="75"/>
+      <c r="B13" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="84">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24">
-        <v>45327</v>
-      </c>
-      <c r="B14" s="38" t="s">
+      <c r="A14" s="75"/>
+      <c r="B14" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="84">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24">
-        <v>45327</v>
-      </c>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="75"/>
+      <c r="B15" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="85">
         <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26">
-        <v>45327</v>
-      </c>
-      <c r="B16" s="40" t="s">
+      <c r="A16" s="76"/>
+      <c r="B16" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="85">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="74">
         <v>45328</v>
       </c>
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="87">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
-        <v>45328</v>
-      </c>
-      <c r="B18" s="52" t="s">
+      <c r="A18" s="75"/>
+      <c r="B18" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="88">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
-        <v>45328</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="75"/>
+      <c r="B19" s="92" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="89">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
-        <v>45328</v>
-      </c>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="75"/>
+      <c r="B20" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="88">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24">
-        <v>45328</v>
-      </c>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="75"/>
+      <c r="B21" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26">
-        <v>45328</v>
-      </c>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="86"/>
+      <c r="B22" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="90">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="79"/>
-      <c r="C23" s="78"/>
+      <c r="A23" s="69">
+        <v>45341</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="63">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="78"/>
+      <c r="A24" s="69">
+        <v>45341</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="64">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="78"/>
+      <c r="A25" s="69">
+        <v>45341</v>
+      </c>
+      <c r="B25" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="68">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="78"/>
+      <c r="A26" s="69">
+        <v>45341</v>
+      </c>
+      <c r="B26" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="68">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="78"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="63"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="78"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="63"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A29" s="69"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="63"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="69"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="63"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="69"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="63"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="63"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="69"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="63"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="63"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="69"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="63"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="63"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="69"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="63"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="69"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="63"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="69"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="63"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="69"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="63"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="69"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="65"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="15">
-        <f>SUM(C8:C29)</f>
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+      <c r="B42" s="12"/>
+      <c r="C42" s="66">
+        <f>SUM(C8:C41)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="18" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A17:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 151&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2592,6 +2826,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005527F882C56960409CF3FB2B047920CD" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07b97e13f27cbcfe17b734c6cbb54e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fec9890b-0385-4b97-bf60-756cae999a32" xmlns:ns3="0628bb02-9a5c-4726-9a61-75fde915aaf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb78319e54262cd22c56c9b99a05c90" ns2:_="" ns3:_="">
     <xsd:import namespace="fec9890b-0385-4b97-bf60-756cae999a32"/>
@@ -2846,27 +3100,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
+    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2883,23 +3136,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
-    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Css et html sur le client
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Git\module-151-Gendres\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DB7322-CCDD-46E9-B9CF-D9DD97D2F6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436490C5-A588-472D-A59E-A1EE28D89810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>Tâches</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>mise en place du login sur le client et le serveur</t>
+  </si>
+  <si>
+    <t>css et logo du client (fait pendant le weekend)</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1275,6 +1278,9 @@
     <xf numFmtId="164" fontId="12" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1323,8 +1329,8 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,8 +1340,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
@@ -1647,80 +1653,80 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="87" t="str">
+      <c r="B3" s="88" t="str">
         <f>'Journal de travail'!B3</f>
         <v xml:space="preserve">Simon Gendre </v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="87">
+      <c r="P3" s="88">
         <v>300633</v>
       </c>
-      <c r="Q3" s="89"/>
+      <c r="Q3" s="90"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="87" t="str">
+      <c r="B4" s="88" t="str">
         <f>'Journal de travail'!B4</f>
         <v>Semaphor</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="90"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1730,32 +1736,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="90" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="91"/>
-      <c r="G7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="90" t="s">
+      <c r="I7" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="91"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="90" t="s">
+      <c r="J7" s="92"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="91"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="90" t="s">
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="93"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1826,7 +1832,7 @@
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="83" t="s">
+      <c r="H9" s="84" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="34" t="s">
@@ -1851,7 +1857,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="35"/>
       <c r="G10" s="36"/>
-      <c r="H10" s="84"/>
+      <c r="H10" s="85"/>
       <c r="I10" s="34"/>
       <c r="J10" s="35"/>
       <c r="K10" s="28"/>
@@ -1872,7 +1878,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="35"/>
       <c r="G11" s="36"/>
-      <c r="H11" s="84"/>
+      <c r="H11" s="85"/>
       <c r="I11" s="34"/>
       <c r="J11" s="35"/>
       <c r="K11" s="28"/>
@@ -1897,7 +1903,7 @@
       <c r="E12" s="34"/>
       <c r="F12" s="35"/>
       <c r="G12" s="36"/>
-      <c r="H12" s="84"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="34"/>
       <c r="J12" s="35"/>
       <c r="K12" s="28"/>
@@ -1922,7 +1928,7 @@
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="84"/>
+      <c r="H13" s="85"/>
       <c r="I13" s="34"/>
       <c r="J13" s="35"/>
       <c r="K13" s="28"/>
@@ -1945,7 +1951,7 @@
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="36"/>
-      <c r="H14" s="84"/>
+      <c r="H14" s="85"/>
       <c r="I14" s="34"/>
       <c r="J14" s="35"/>
       <c r="K14" s="28"/>
@@ -1968,7 +1974,7 @@
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="36"/>
-      <c r="H15" s="84"/>
+      <c r="H15" s="85"/>
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
       <c r="K15" s="28"/>
@@ -1993,7 +1999,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="36"/>
-      <c r="H16" s="84"/>
+      <c r="H16" s="85"/>
       <c r="I16" s="34"/>
       <c r="J16" s="35"/>
       <c r="K16" s="28"/>
@@ -2016,7 +2022,7 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="84"/>
+      <c r="H17" s="85"/>
       <c r="I17" s="34"/>
       <c r="J17" s="35"/>
       <c r="K17" s="28"/>
@@ -2037,7 +2043,7 @@
       <c r="E18" s="34"/>
       <c r="F18" s="35"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="84"/>
+      <c r="H18" s="85"/>
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
       <c r="K18" s="28"/>
@@ -2058,7 +2064,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="40"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="84"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
       <c r="K19" s="28"/>
@@ -2081,7 +2087,7 @@
       <c r="G20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="84"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="34"/>
       <c r="J20" s="35"/>
       <c r="K20" s="28" t="s">
@@ -2106,7 +2112,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="36"/>
-      <c r="H21" s="84"/>
+      <c r="H21" s="85"/>
       <c r="I21" s="42"/>
       <c r="J21" s="35"/>
       <c r="K21" s="28"/>
@@ -2129,7 +2135,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="36"/>
-      <c r="H22" s="84"/>
+      <c r="H22" s="85"/>
       <c r="I22" s="42" t="s">
         <v>60</v>
       </c>
@@ -2154,7 +2160,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="35"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="84"/>
+      <c r="H23" s="85"/>
       <c r="I23" s="34"/>
       <c r="J23" s="35"/>
       <c r="K23" s="28"/>
@@ -2175,7 +2181,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="35"/>
       <c r="G24" s="43"/>
-      <c r="H24" s="84"/>
+      <c r="H24" s="85"/>
       <c r="I24" s="34" t="s">
         <v>60</v>
       </c>
@@ -2198,7 +2204,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="35"/>
       <c r="G25" s="36"/>
-      <c r="H25" s="84"/>
+      <c r="H25" s="85"/>
       <c r="I25" s="44"/>
       <c r="J25" s="35"/>
       <c r="K25" s="28" t="s">
@@ -2221,7 +2227,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="35"/>
       <c r="G26" s="36"/>
-      <c r="H26" s="84"/>
+      <c r="H26" s="85"/>
       <c r="I26" s="34"/>
       <c r="J26" s="45"/>
       <c r="K26" s="28"/>
@@ -2242,7 +2248,7 @@
       <c r="E27" s="34"/>
       <c r="F27" s="35"/>
       <c r="G27" s="36"/>
-      <c r="H27" s="84"/>
+      <c r="H27" s="85"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
       <c r="K27" s="29"/>
@@ -2263,7 +2269,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="35"/>
       <c r="G28" s="36"/>
-      <c r="H28" s="84"/>
+      <c r="H28" s="85"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
       <c r="K28" s="28"/>
@@ -2284,7 +2290,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="35"/>
       <c r="G29" s="43"/>
-      <c r="H29" s="84"/>
+      <c r="H29" s="85"/>
       <c r="I29" s="34" t="s">
         <v>60</v>
       </c>
@@ -2309,7 +2315,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="35"/>
       <c r="G30" s="36"/>
-      <c r="H30" s="84"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="44"/>
       <c r="J30" s="35" t="s">
         <v>60</v>
@@ -2334,7 +2340,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="35"/>
       <c r="G31" s="36"/>
-      <c r="H31" s="84"/>
+      <c r="H31" s="85"/>
       <c r="I31" s="34"/>
       <c r="J31" s="45"/>
       <c r="K31" s="28"/>
@@ -2355,7 +2361,7 @@
       <c r="E32" s="34"/>
       <c r="F32" s="35"/>
       <c r="G32" s="36"/>
-      <c r="H32" s="84"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
       <c r="K32" s="29"/>
@@ -2376,7 +2382,7 @@
       <c r="E33" s="34"/>
       <c r="F33" s="35"/>
       <c r="G33" s="36"/>
-      <c r="H33" s="84"/>
+      <c r="H33" s="85"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
       <c r="K33" s="28"/>
@@ -2397,7 +2403,7 @@
       <c r="E34" s="34"/>
       <c r="F34" s="35"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="84"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
       <c r="K34" s="28"/>
@@ -2418,7 +2424,7 @@
       <c r="E35" s="34"/>
       <c r="F35" s="35"/>
       <c r="G35" s="36"/>
-      <c r="H35" s="84"/>
+      <c r="H35" s="85"/>
       <c r="I35" s="34"/>
       <c r="J35" s="35"/>
       <c r="K35" s="28"/>
@@ -2439,7 +2445,7 @@
       <c r="E36" s="34"/>
       <c r="F36" s="35"/>
       <c r="G36" s="36"/>
-      <c r="H36" s="84"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="34"/>
       <c r="J36" s="35"/>
       <c r="K36" s="28"/>
@@ -2458,7 +2464,7 @@
       <c r="E37" s="34"/>
       <c r="F37" s="35"/>
       <c r="G37" s="36"/>
-      <c r="H37" s="84"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="34"/>
       <c r="J37" s="35"/>
       <c r="K37" s="28"/>
@@ -2477,7 +2483,7 @@
       <c r="E38" s="47"/>
       <c r="F38" s="48"/>
       <c r="G38" s="49"/>
-      <c r="H38" s="85"/>
+      <c r="H38" s="86"/>
       <c r="I38" s="47"/>
       <c r="J38" s="48"/>
       <c r="K38" s="30"/>
@@ -2521,10 +2527,10 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
@@ -2532,11 +2538,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2591,7 +2597,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="93">
+      <c r="A10" s="94">
         <v>45327</v>
       </c>
       <c r="B10" s="63" t="s">
@@ -2602,7 +2608,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
+      <c r="A11" s="95"/>
       <c r="B11" s="64" t="s">
         <v>62</v>
       </c>
@@ -2611,7 +2617,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="95"/>
       <c r="B12" s="64" t="s">
         <v>63</v>
       </c>
@@ -2620,7 +2626,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
+      <c r="A13" s="95"/>
       <c r="B13" s="64" t="s">
         <v>53</v>
       </c>
@@ -2629,7 +2635,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
+      <c r="A14" s="95"/>
       <c r="B14" s="64" t="s">
         <v>74</v>
       </c>
@@ -2638,7 +2644,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="65" t="s">
         <v>75</v>
       </c>
@@ -2647,7 +2653,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="95"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="65" t="s">
         <v>57</v>
       </c>
@@ -2656,7 +2662,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="93">
+      <c r="A17" s="94">
         <v>45328</v>
       </c>
       <c r="B17" s="73" t="s">
@@ -2667,7 +2673,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
+      <c r="A18" s="95"/>
       <c r="B18" s="62" t="s">
         <v>78</v>
       </c>
@@ -2676,7 +2682,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
+      <c r="A19" s="95"/>
       <c r="B19" s="74" t="s">
         <v>79</v>
       </c>
@@ -2685,7 +2691,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
+      <c r="A20" s="95"/>
       <c r="B20" s="62" t="s">
         <v>80</v>
       </c>
@@ -2694,7 +2700,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
+      <c r="A21" s="95"/>
       <c r="B21" s="62" t="s">
         <v>81</v>
       </c>
@@ -2703,7 +2709,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="94"/>
+      <c r="A22" s="95"/>
       <c r="B22" s="75" t="s">
         <v>82</v>
       </c>
@@ -2712,7 +2718,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="96">
+      <c r="A23" s="97">
         <v>45341</v>
       </c>
       <c r="B23" s="78" t="s">
@@ -2723,7 +2729,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="97"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="51" t="s">
         <v>84</v>
       </c>
@@ -2732,7 +2738,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="97"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="55" t="s">
         <v>85</v>
       </c>
@@ -2741,7 +2747,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="97"/>
+      <c r="A26" s="98"/>
       <c r="B26" s="55" t="s">
         <v>86</v>
       </c>
@@ -2750,7 +2756,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="97"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="50" t="s">
         <v>87</v>
       </c>
@@ -2759,7 +2765,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="98"/>
+      <c r="A28" s="99"/>
       <c r="B28" s="81" t="s">
         <v>88</v>
       </c>
@@ -2768,10 +2774,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="93">
+      <c r="A29" s="94">
         <v>45342</v>
       </c>
-      <c r="B29" s="99" t="s">
+      <c r="B29" s="83" t="s">
         <v>79</v>
       </c>
       <c r="C29" s="79">
@@ -2779,7 +2785,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="51" t="s">
         <v>89</v>
       </c>
@@ -2788,7 +2794,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="94"/>
+      <c r="A31" s="95"/>
       <c r="B31" s="55" t="s">
         <v>90</v>
       </c>
@@ -2797,7 +2803,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="95"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="81" t="s">
         <v>91</v>
       </c>
@@ -2806,9 +2812,15 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="52"/>
+      <c r="A33" s="77">
+        <v>45346</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="100">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="56"/>
@@ -2857,7 +2869,7 @@
       <c r="B42" s="12"/>
       <c r="C42" s="54">
         <f>SUM(C8:C41)</f>
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2899,7 +2911,7 @@
     <mergeCell ref="A29:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 151&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2908,26 +2920,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005527F882C56960409CF3FB2B047920CD" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07b97e13f27cbcfe17b734c6cbb54e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fec9890b-0385-4b97-bf60-756cae999a32" xmlns:ns3="0628bb02-9a5c-4726-9a61-75fde915aaf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb78319e54262cd22c56c9b99a05c90" ns2:_="" ns3:_="">
     <xsd:import namespace="fec9890b-0385-4b97-bf60-756cae999a32"/>
@@ -3182,10 +3174,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
+    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3202,20 +3225,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
-    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
les message peuvent etre envoyés
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Git\module-151-Gendres\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436490C5-A588-472D-A59E-A1EE28D89810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F24F8E-8C6C-46FC-83E5-8D78087AF08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>Tâches</t>
   </si>
@@ -411,6 +411,18 @@
   </si>
   <si>
     <t>css et logo du client (fait pendant le weekend)</t>
+  </si>
+  <si>
+    <t>mise en place de la récuperation de messages dans la DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mise en place de la déconnexion </t>
+  </si>
+  <si>
+    <t>mise en place de l'envoie de message (coté serveur)</t>
+  </si>
+  <si>
+    <t>mise en place de l'envoie de message (coté client)</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1066,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1281,6 +1293,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1311,6 +1335,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1318,18 +1351,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1649,84 +1670,84 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A9" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="92" t="str">
         <f>'Journal de travail'!B3</f>
         <v xml:space="preserve">Simon Gendre </v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="94"/>
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="88">
+      <c r="P3" s="92">
         <v>300633</v>
       </c>
-      <c r="Q3" s="90"/>
+      <c r="Q3" s="94"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="88" t="str">
+      <c r="B4" s="92" t="str">
         <f>'Journal de travail'!B4</f>
         <v>Semaphor</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="90"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="94"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1736,32 +1757,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="91" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="92"/>
-      <c r="G7" s="93"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="97"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="91" t="s">
+      <c r="I7" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="92"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="91" t="s">
+      <c r="J7" s="96"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="92"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="91" t="s">
+      <c r="M7" s="96"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="93"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="97"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1832,7 +1853,7 @@
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="88" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="34" t="s">
@@ -1857,7 +1878,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="35"/>
       <c r="G10" s="36"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="89"/>
       <c r="I10" s="34"/>
       <c r="J10" s="35"/>
       <c r="K10" s="28"/>
@@ -1878,7 +1899,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="35"/>
       <c r="G11" s="36"/>
-      <c r="H11" s="85"/>
+      <c r="H11" s="89"/>
       <c r="I11" s="34"/>
       <c r="J11" s="35"/>
       <c r="K11" s="28"/>
@@ -1903,7 +1924,7 @@
       <c r="E12" s="34"/>
       <c r="F12" s="35"/>
       <c r="G12" s="36"/>
-      <c r="H12" s="85"/>
+      <c r="H12" s="89"/>
       <c r="I12" s="34"/>
       <c r="J12" s="35"/>
       <c r="K12" s="28"/>
@@ -1928,7 +1949,7 @@
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="85"/>
+      <c r="H13" s="89"/>
       <c r="I13" s="34"/>
       <c r="J13" s="35"/>
       <c r="K13" s="28"/>
@@ -1951,7 +1972,7 @@
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="36"/>
-      <c r="H14" s="85"/>
+      <c r="H14" s="89"/>
       <c r="I14" s="34"/>
       <c r="J14" s="35"/>
       <c r="K14" s="28"/>
@@ -1974,7 +1995,7 @@
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="36"/>
-      <c r="H15" s="85"/>
+      <c r="H15" s="89"/>
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
       <c r="K15" s="28"/>
@@ -1999,7 +2020,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="36"/>
-      <c r="H16" s="85"/>
+      <c r="H16" s="89"/>
       <c r="I16" s="34"/>
       <c r="J16" s="35"/>
       <c r="K16" s="28"/>
@@ -2022,7 +2043,7 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="85"/>
+      <c r="H17" s="89"/>
       <c r="I17" s="34"/>
       <c r="J17" s="35"/>
       <c r="K17" s="28"/>
@@ -2043,7 +2064,7 @@
       <c r="E18" s="34"/>
       <c r="F18" s="35"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="85"/>
+      <c r="H18" s="89"/>
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
       <c r="K18" s="28"/>
@@ -2064,7 +2085,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="40"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="85"/>
+      <c r="H19" s="89"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
       <c r="K19" s="28"/>
@@ -2087,7 +2108,7 @@
       <c r="G20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="85"/>
+      <c r="H20" s="89"/>
       <c r="I20" s="34"/>
       <c r="J20" s="35"/>
       <c r="K20" s="28" t="s">
@@ -2112,7 +2133,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="36"/>
-      <c r="H21" s="85"/>
+      <c r="H21" s="89"/>
       <c r="I21" s="42"/>
       <c r="J21" s="35"/>
       <c r="K21" s="28"/>
@@ -2135,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="36"/>
-      <c r="H22" s="85"/>
+      <c r="H22" s="89"/>
       <c r="I22" s="42" t="s">
         <v>60</v>
       </c>
@@ -2160,7 +2181,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="35"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="85"/>
+      <c r="H23" s="89"/>
       <c r="I23" s="34"/>
       <c r="J23" s="35"/>
       <c r="K23" s="28"/>
@@ -2181,7 +2202,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="35"/>
       <c r="G24" s="43"/>
-      <c r="H24" s="85"/>
+      <c r="H24" s="89"/>
       <c r="I24" s="34" t="s">
         <v>60</v>
       </c>
@@ -2204,7 +2225,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="35"/>
       <c r="G25" s="36"/>
-      <c r="H25" s="85"/>
+      <c r="H25" s="89"/>
       <c r="I25" s="44"/>
       <c r="J25" s="35"/>
       <c r="K25" s="28" t="s">
@@ -2227,11 +2248,13 @@
       <c r="E26" s="34"/>
       <c r="F26" s="35"/>
       <c r="G26" s="36"/>
-      <c r="H26" s="85"/>
+      <c r="H26" s="89"/>
       <c r="I26" s="34"/>
       <c r="J26" s="45"/>
       <c r="K26" s="28"/>
-      <c r="L26" s="34"/>
+      <c r="L26" s="34" t="s">
+        <v>60</v>
+      </c>
       <c r="M26" s="35"/>
       <c r="N26" s="36"/>
       <c r="O26" s="34"/>
@@ -2248,11 +2271,13 @@
       <c r="E27" s="34"/>
       <c r="F27" s="35"/>
       <c r="G27" s="36"/>
-      <c r="H27" s="85"/>
+      <c r="H27" s="89"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
       <c r="K27" s="29"/>
-      <c r="L27" s="34"/>
+      <c r="L27" s="34" t="s">
+        <v>60</v>
+      </c>
       <c r="M27" s="35"/>
       <c r="N27" s="36"/>
       <c r="O27" s="34"/>
@@ -2269,7 +2294,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="35"/>
       <c r="G28" s="36"/>
-      <c r="H28" s="85"/>
+      <c r="H28" s="89"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
       <c r="K28" s="28"/>
@@ -2290,7 +2315,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="35"/>
       <c r="G29" s="43"/>
-      <c r="H29" s="85"/>
+      <c r="H29" s="89"/>
       <c r="I29" s="34" t="s">
         <v>60</v>
       </c>
@@ -2315,7 +2340,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="35"/>
       <c r="G30" s="36"/>
-      <c r="H30" s="85"/>
+      <c r="H30" s="89"/>
       <c r="I30" s="44"/>
       <c r="J30" s="35" t="s">
         <v>60</v>
@@ -2340,11 +2365,13 @@
       <c r="E31" s="34"/>
       <c r="F31" s="35"/>
       <c r="G31" s="36"/>
-      <c r="H31" s="85"/>
+      <c r="H31" s="89"/>
       <c r="I31" s="34"/>
       <c r="J31" s="45"/>
       <c r="K31" s="28"/>
-      <c r="L31" s="34"/>
+      <c r="L31" s="34" t="s">
+        <v>60</v>
+      </c>
       <c r="M31" s="35"/>
       <c r="N31" s="36"/>
       <c r="O31" s="34"/>
@@ -2361,11 +2388,13 @@
       <c r="E32" s="34"/>
       <c r="F32" s="35"/>
       <c r="G32" s="36"/>
-      <c r="H32" s="85"/>
+      <c r="H32" s="89"/>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="34"/>
+      <c r="L32" s="34" t="s">
+        <v>60</v>
+      </c>
       <c r="M32" s="35"/>
       <c r="N32" s="36"/>
       <c r="O32" s="34"/>
@@ -2382,7 +2411,7 @@
       <c r="E33" s="34"/>
       <c r="F33" s="35"/>
       <c r="G33" s="36"/>
-      <c r="H33" s="85"/>
+      <c r="H33" s="89"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
       <c r="K33" s="28"/>
@@ -2403,7 +2432,7 @@
       <c r="E34" s="34"/>
       <c r="F34" s="35"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="85"/>
+      <c r="H34" s="89"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
       <c r="K34" s="28"/>
@@ -2424,7 +2453,7 @@
       <c r="E35" s="34"/>
       <c r="F35" s="35"/>
       <c r="G35" s="36"/>
-      <c r="H35" s="85"/>
+      <c r="H35" s="89"/>
       <c r="I35" s="34"/>
       <c r="J35" s="35"/>
       <c r="K35" s="28"/>
@@ -2445,7 +2474,7 @@
       <c r="E36" s="34"/>
       <c r="F36" s="35"/>
       <c r="G36" s="36"/>
-      <c r="H36" s="85"/>
+      <c r="H36" s="89"/>
       <c r="I36" s="34"/>
       <c r="J36" s="35"/>
       <c r="K36" s="28"/>
@@ -2464,7 +2493,7 @@
       <c r="E37" s="34"/>
       <c r="F37" s="35"/>
       <c r="G37" s="36"/>
-      <c r="H37" s="85"/>
+      <c r="H37" s="89"/>
       <c r="I37" s="34"/>
       <c r="J37" s="35"/>
       <c r="K37" s="28"/>
@@ -2483,7 +2512,7 @@
       <c r="E38" s="47"/>
       <c r="F38" s="48"/>
       <c r="G38" s="49"/>
-      <c r="H38" s="86"/>
+      <c r="H38" s="90"/>
       <c r="I38" s="47"/>
       <c r="J38" s="48"/>
       <c r="K38" s="30"/>
@@ -2526,11 +2555,11 @@
   </sheetPr>
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
@@ -2538,11 +2567,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2597,7 +2626,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="94">
+      <c r="A10" s="101">
         <v>45327</v>
       </c>
       <c r="B10" s="63" t="s">
@@ -2608,7 +2637,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="95"/>
+      <c r="A11" s="102"/>
       <c r="B11" s="64" t="s">
         <v>62</v>
       </c>
@@ -2617,7 +2646,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
+      <c r="A12" s="102"/>
       <c r="B12" s="64" t="s">
         <v>63</v>
       </c>
@@ -2626,7 +2655,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
+      <c r="A13" s="102"/>
       <c r="B13" s="64" t="s">
         <v>53</v>
       </c>
@@ -2635,7 +2664,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
+      <c r="A14" s="102"/>
       <c r="B14" s="64" t="s">
         <v>74</v>
       </c>
@@ -2644,7 +2673,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
+      <c r="A15" s="102"/>
       <c r="B15" s="65" t="s">
         <v>75</v>
       </c>
@@ -2653,7 +2682,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="96"/>
+      <c r="A16" s="103"/>
       <c r="B16" s="65" t="s">
         <v>57</v>
       </c>
@@ -2662,7 +2691,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="94">
+      <c r="A17" s="101">
         <v>45328</v>
       </c>
       <c r="B17" s="73" t="s">
@@ -2673,7 +2702,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
+      <c r="A18" s="102"/>
       <c r="B18" s="62" t="s">
         <v>78</v>
       </c>
@@ -2682,7 +2711,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
+      <c r="A19" s="102"/>
       <c r="B19" s="74" t="s">
         <v>79</v>
       </c>
@@ -2691,7 +2720,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
+      <c r="A20" s="102"/>
       <c r="B20" s="62" t="s">
         <v>80</v>
       </c>
@@ -2700,7 +2729,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
+      <c r="A21" s="102"/>
       <c r="B21" s="62" t="s">
         <v>81</v>
       </c>
@@ -2709,7 +2738,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95"/>
+      <c r="A22" s="102"/>
       <c r="B22" s="75" t="s">
         <v>82</v>
       </c>
@@ -2718,7 +2747,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="97">
+      <c r="A23" s="98">
         <v>45341</v>
       </c>
       <c r="B23" s="78" t="s">
@@ -2729,7 +2758,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="51" t="s">
         <v>84</v>
       </c>
@@ -2738,7 +2767,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
+      <c r="A25" s="99"/>
       <c r="B25" s="55" t="s">
         <v>85</v>
       </c>
@@ -2747,7 +2776,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="98"/>
+      <c r="A26" s="99"/>
       <c r="B26" s="55" t="s">
         <v>86</v>
       </c>
@@ -2756,7 +2785,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
+      <c r="A27" s="99"/>
       <c r="B27" s="50" t="s">
         <v>87</v>
       </c>
@@ -2765,7 +2794,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="99"/>
+      <c r="A28" s="100"/>
       <c r="B28" s="81" t="s">
         <v>88</v>
       </c>
@@ -2774,7 +2803,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="94">
+      <c r="A29" s="101">
         <v>45342</v>
       </c>
       <c r="B29" s="83" t="s">
@@ -2785,7 +2814,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
+      <c r="A30" s="102"/>
       <c r="B30" s="51" t="s">
         <v>89</v>
       </c>
@@ -2794,7 +2823,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
+      <c r="A31" s="102"/>
       <c r="B31" s="55" t="s">
         <v>90</v>
       </c>
@@ -2803,7 +2832,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="96"/>
+      <c r="A32" s="103"/>
       <c r="B32" s="81" t="s">
         <v>91</v>
       </c>
@@ -2811,39 +2840,57 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="77">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="58">
         <v>45346</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="100">
+      <c r="C33" s="85">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="52"/>
+      <c r="A34" s="98">
+        <v>45348</v>
+      </c>
+      <c r="B34" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="87">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="52"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="80">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="52"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="52"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="100"/>
+      <c r="B37" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="82">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
+      <c r="A38" s="77"/>
       <c r="B38" s="50"/>
       <c r="C38" s="52"/>
     </row>
@@ -2869,7 +2916,7 @@
       <c r="B42" s="12"/>
       <c r="C42" s="54">
         <f>SUM(C8:C41)</f>
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2903,7 +2950,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A34:A37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A22"/>

</xml_diff>

<commit_message>
ajout de la creation de compte et correction de bugs
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F24F8E-8C6C-46FC-83E5-8D78087AF08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBA4ECE-3995-4142-9AE9-573732AA6347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
   <si>
     <t>Tâches</t>
   </si>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t>mise en place de l'envoie de message (coté client)</t>
+  </si>
+  <si>
+    <t>Serveur - création de comptes</t>
+  </si>
+  <si>
+    <t>Client -  - création de comptes</t>
+  </si>
+  <si>
+    <t>implémentation de la création de comptes (client et serveur)</t>
+  </si>
+  <si>
+    <t>Correction de bugs sur le client</t>
   </si>
 </sst>
 </file>
@@ -585,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1062,11 +1074,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1352,6 +1373,15 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1668,10 +1698,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2308,9 @@
       <c r="L27" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="M27" s="35"/>
+      <c r="M27" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="N27" s="36"/>
       <c r="O27" s="34"/>
       <c r="P27" s="35"/>
@@ -2286,7 +2318,7 @@
     </row>
     <row r="28" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="35"/>
@@ -2297,57 +2329,55 @@
       <c r="H28" s="89"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
-      <c r="K28" s="28"/>
+      <c r="K28" s="29"/>
       <c r="L28" s="34"/>
       <c r="M28" s="45"/>
-      <c r="N28" s="43"/>
+      <c r="N28" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="O28" s="34"/>
       <c r="P28" s="35"/>
       <c r="Q28" s="36"/>
     </row>
     <row r="29" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
       <c r="E29" s="34"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="43"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="89"/>
-      <c r="I29" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="J29" s="35" t="s">
-        <v>60</v>
-      </c>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
       <c r="K29" s="28"/>
       <c r="L29" s="34"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="36"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="43"/>
       <c r="O29" s="34"/>
       <c r="P29" s="35"/>
       <c r="Q29" s="36"/>
     </row>
     <row r="30" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="34"/>
       <c r="C30" s="35"/>
       <c r="D30" s="36"/>
       <c r="E30" s="34"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="89"/>
-      <c r="I30" s="44"/>
+      <c r="I30" s="34" t="s">
+        <v>60</v>
+      </c>
       <c r="J30" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="K30" s="28" t="s">
-        <v>60</v>
-      </c>
+      <c r="K30" s="28"/>
       <c r="L30" s="34"/>
       <c r="M30" s="35"/>
       <c r="N30" s="36"/>
@@ -2357,7 +2387,7 @@
     </row>
     <row r="31" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="35"/>
@@ -2366,12 +2396,14 @@
       <c r="F31" s="35"/>
       <c r="G31" s="36"/>
       <c r="H31" s="89"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="34" t="s">
+      <c r="I31" s="44"/>
+      <c r="J31" s="35" t="s">
         <v>60</v>
       </c>
+      <c r="K31" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" s="34"/>
       <c r="M31" s="35"/>
       <c r="N31" s="36"/>
       <c r="O31" s="34"/>
@@ -2380,7 +2412,7 @@
     </row>
     <row r="32" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="35"/>
@@ -2390,8 +2422,8 @@
       <c r="G32" s="36"/>
       <c r="H32" s="89"/>
       <c r="I32" s="34"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="29"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="34" t="s">
         <v>60</v>
       </c>
@@ -2403,7 +2435,7 @@
     </row>
     <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="35"/>
@@ -2413,18 +2445,20 @@
       <c r="G33" s="36"/>
       <c r="H33" s="89"/>
       <c r="I33" s="34"/>
-      <c r="J33" s="35"/>
+      <c r="J33" s="45"/>
       <c r="K33" s="28"/>
       <c r="L33" s="34"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="43"/>
+      <c r="N33" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="O33" s="34"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="36"/>
     </row>
     <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B34" s="34"/>
       <c r="C34" s="35"/>
@@ -2435,17 +2469,21 @@
       <c r="H34" s="89"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="35"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="N34" s="36"/>
       <c r="O34" s="34"/>
-      <c r="P34" s="45"/>
+      <c r="P34" s="35"/>
       <c r="Q34" s="36"/>
     </row>
     <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B35" s="34"/>
       <c r="C35" s="35"/>
@@ -2458,15 +2496,15 @@
       <c r="J35" s="35"/>
       <c r="K35" s="28"/>
       <c r="L35" s="34"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="36"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="43"/>
       <c r="O35" s="34"/>
       <c r="P35" s="35"/>
-      <c r="Q35" s="43"/>
+      <c r="Q35" s="36"/>
     </row>
     <row r="36" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>15</v>
+      <c r="A36" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="B36" s="34"/>
       <c r="C36" s="35"/>
@@ -2478,15 +2516,17 @@
       <c r="I36" s="34"/>
       <c r="J36" s="35"/>
       <c r="K36" s="28"/>
-      <c r="L36" s="46"/>
+      <c r="L36" s="34"/>
       <c r="M36" s="35"/>
       <c r="N36" s="36"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="35"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="45"/>
       <c r="Q36" s="36"/>
     </row>
     <row r="37" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="A37" s="26" t="s">
+        <v>58</v>
+      </c>
       <c r="B37" s="34"/>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
@@ -2502,33 +2542,73 @@
       <c r="N37" s="36"/>
       <c r="O37" s="34"/>
       <c r="P37" s="35"/>
-      <c r="Q37" s="36"/>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="90"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="49"/>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
+      <c r="Q37" s="43"/>
+    </row>
+    <row r="38" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="36"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="36"/>
+    </row>
+    <row r="39" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="34"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="36"/>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="90"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="48"/>
+      <c r="Q40" s="49"/>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="H9:H38"/>
+    <mergeCell ref="H9:H40"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:M4"/>
@@ -2553,10 +2633,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,76 +2961,106 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="81" t="s">
+      <c r="A37" s="99"/>
+      <c r="B37" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="82">
+      <c r="C37" s="80">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="52"/>
+      <c r="A38" s="101">
+        <v>45349</v>
+      </c>
+      <c r="B38" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="87">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="52"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="52"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="72">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="103"/>
+      <c r="B40" s="106" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="82">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="53"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A41" s="77"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="52"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="56"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="52"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="52"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="53"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="54">
-        <f>SUM(C8:C41)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="12"/>
+      <c r="C45" s="54">
+        <f>SUM(C8:C44)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="16" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="17" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A10:A16"/>
@@ -2968,6 +3078,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005527F882C56960409CF3FB2B047920CD" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07b97e13f27cbcfe17b734c6cbb54e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fec9890b-0385-4b97-bf60-756cae999a32" xmlns:ns3="0628bb02-9a5c-4726-9a61-75fde915aaf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb78319e54262cd22c56c9b99a05c90" ns2:_="" ns3:_="">
     <xsd:import namespace="fec9890b-0385-4b97-bf60-756cae999a32"/>
@@ -3222,27 +3352,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
+    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3259,23 +3388,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
-    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update 151 - planning et journal - GENDRE.xlsx
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Git\module-151-Gendres\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBA4ECE-3995-4142-9AE9-573732AA6347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17BB562-FA29-4244-B16E-DE4BB6E1CF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="103">
   <si>
     <t>Tâches</t>
   </si>
@@ -435,6 +435,12 @@
   </si>
   <si>
     <t>Correction de bugs sur le client</t>
+  </si>
+  <si>
+    <t>optimisisation du code</t>
+  </si>
+  <si>
+    <t>ajout du mode admin (weekend)</t>
   </si>
 </sst>
 </file>
@@ -1326,6 +1332,15 @@
     <xf numFmtId="164" fontId="12" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1356,6 +1371,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1364,24 +1388,6 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1704,80 +1710,80 @@
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="92" t="str">
+      <c r="B3" s="95" t="str">
         <f>'Journal de travail'!B3</f>
         <v xml:space="preserve">Simon Gendre </v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="94"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="97"/>
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="92">
+      <c r="P3" s="95">
         <v>300633</v>
       </c>
-      <c r="Q3" s="94"/>
+      <c r="Q3" s="97"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="92" t="str">
+      <c r="B4" s="95" t="str">
         <f>'Journal de travail'!B4</f>
         <v>Semaphor</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="94"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="97"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1787,32 +1793,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="95" t="s">
+      <c r="C7" s="99"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="96"/>
-      <c r="G7" s="97"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="100"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="95" t="s">
+      <c r="J7" s="99"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="96"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="95" t="s">
+      <c r="M7" s="99"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="97"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="100"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1883,7 +1889,7 @@
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="88" t="s">
+      <c r="H9" s="91" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="34" t="s">
@@ -1908,7 +1914,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="35"/>
       <c r="G10" s="36"/>
-      <c r="H10" s="89"/>
+      <c r="H10" s="92"/>
       <c r="I10" s="34"/>
       <c r="J10" s="35"/>
       <c r="K10" s="28"/>
@@ -1929,7 +1935,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="35"/>
       <c r="G11" s="36"/>
-      <c r="H11" s="89"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="34"/>
       <c r="J11" s="35"/>
       <c r="K11" s="28"/>
@@ -1954,7 +1960,7 @@
       <c r="E12" s="34"/>
       <c r="F12" s="35"/>
       <c r="G12" s="36"/>
-      <c r="H12" s="89"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="34"/>
       <c r="J12" s="35"/>
       <c r="K12" s="28"/>
@@ -1979,7 +1985,7 @@
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="89"/>
+      <c r="H13" s="92"/>
       <c r="I13" s="34"/>
       <c r="J13" s="35"/>
       <c r="K13" s="28"/>
@@ -2002,7 +2008,7 @@
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="36"/>
-      <c r="H14" s="89"/>
+      <c r="H14" s="92"/>
       <c r="I14" s="34"/>
       <c r="J14" s="35"/>
       <c r="K14" s="28"/>
@@ -2025,7 +2031,7 @@
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="36"/>
-      <c r="H15" s="89"/>
+      <c r="H15" s="92"/>
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
       <c r="K15" s="28"/>
@@ -2050,7 +2056,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="36"/>
-      <c r="H16" s="89"/>
+      <c r="H16" s="92"/>
       <c r="I16" s="34"/>
       <c r="J16" s="35"/>
       <c r="K16" s="28"/>
@@ -2073,7 +2079,7 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="89"/>
+      <c r="H17" s="92"/>
       <c r="I17" s="34"/>
       <c r="J17" s="35"/>
       <c r="K17" s="28"/>
@@ -2094,7 +2100,7 @@
       <c r="E18" s="34"/>
       <c r="F18" s="35"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="89"/>
+      <c r="H18" s="92"/>
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
       <c r="K18" s="28"/>
@@ -2115,7 +2121,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="40"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="89"/>
+      <c r="H19" s="92"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
       <c r="K19" s="28"/>
@@ -2138,7 +2144,7 @@
       <c r="G20" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="89"/>
+      <c r="H20" s="92"/>
       <c r="I20" s="34"/>
       <c r="J20" s="35"/>
       <c r="K20" s="28" t="s">
@@ -2163,7 +2169,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="36"/>
-      <c r="H21" s="89"/>
+      <c r="H21" s="92"/>
       <c r="I21" s="42"/>
       <c r="J21" s="35"/>
       <c r="K21" s="28"/>
@@ -2186,7 +2192,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="36"/>
-      <c r="H22" s="89"/>
+      <c r="H22" s="92"/>
       <c r="I22" s="42" t="s">
         <v>60</v>
       </c>
@@ -2211,7 +2217,7 @@
       <c r="E23" s="34"/>
       <c r="F23" s="35"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="89"/>
+      <c r="H23" s="92"/>
       <c r="I23" s="34"/>
       <c r="J23" s="35"/>
       <c r="K23" s="28"/>
@@ -2232,7 +2238,7 @@
       <c r="E24" s="34"/>
       <c r="F24" s="35"/>
       <c r="G24" s="43"/>
-      <c r="H24" s="89"/>
+      <c r="H24" s="92"/>
       <c r="I24" s="34" t="s">
         <v>60</v>
       </c>
@@ -2255,7 +2261,7 @@
       <c r="E25" s="34"/>
       <c r="F25" s="35"/>
       <c r="G25" s="36"/>
-      <c r="H25" s="89"/>
+      <c r="H25" s="92"/>
       <c r="I25" s="44"/>
       <c r="J25" s="35"/>
       <c r="K25" s="28" t="s">
@@ -2278,7 +2284,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="35"/>
       <c r="G26" s="36"/>
-      <c r="H26" s="89"/>
+      <c r="H26" s="92"/>
       <c r="I26" s="34"/>
       <c r="J26" s="45"/>
       <c r="K26" s="28"/>
@@ -2301,7 +2307,7 @@
       <c r="E27" s="34"/>
       <c r="F27" s="35"/>
       <c r="G27" s="36"/>
-      <c r="H27" s="89"/>
+      <c r="H27" s="92"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
       <c r="K27" s="29"/>
@@ -2326,7 +2332,7 @@
       <c r="E28" s="34"/>
       <c r="F28" s="35"/>
       <c r="G28" s="36"/>
-      <c r="H28" s="89"/>
+      <c r="H28" s="92"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
       <c r="K28" s="29"/>
@@ -2349,7 +2355,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="35"/>
       <c r="G29" s="36"/>
-      <c r="H29" s="89"/>
+      <c r="H29" s="92"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
       <c r="K29" s="28"/>
@@ -2370,7 +2376,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="35"/>
       <c r="G30" s="43"/>
-      <c r="H30" s="89"/>
+      <c r="H30" s="92"/>
       <c r="I30" s="34" t="s">
         <v>60</v>
       </c>
@@ -2395,7 +2401,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="35"/>
       <c r="G31" s="36"/>
-      <c r="H31" s="89"/>
+      <c r="H31" s="92"/>
       <c r="I31" s="44"/>
       <c r="J31" s="35" t="s">
         <v>60</v>
@@ -2420,7 +2426,7 @@
       <c r="E32" s="34"/>
       <c r="F32" s="35"/>
       <c r="G32" s="36"/>
-      <c r="H32" s="89"/>
+      <c r="H32" s="92"/>
       <c r="I32" s="34"/>
       <c r="J32" s="45"/>
       <c r="K32" s="28"/>
@@ -2443,7 +2449,7 @@
       <c r="E33" s="34"/>
       <c r="F33" s="35"/>
       <c r="G33" s="36"/>
-      <c r="H33" s="89"/>
+      <c r="H33" s="92"/>
       <c r="I33" s="34"/>
       <c r="J33" s="45"/>
       <c r="K33" s="28"/>
@@ -2466,7 +2472,7 @@
       <c r="E34" s="34"/>
       <c r="F34" s="35"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="89"/>
+      <c r="H34" s="92"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
       <c r="K34" s="29"/>
@@ -2491,7 +2497,7 @@
       <c r="E35" s="34"/>
       <c r="F35" s="35"/>
       <c r="G35" s="36"/>
-      <c r="H35" s="89"/>
+      <c r="H35" s="92"/>
       <c r="I35" s="34"/>
       <c r="J35" s="35"/>
       <c r="K35" s="28"/>
@@ -2512,7 +2518,7 @@
       <c r="E36" s="34"/>
       <c r="F36" s="35"/>
       <c r="G36" s="36"/>
-      <c r="H36" s="89"/>
+      <c r="H36" s="92"/>
       <c r="I36" s="34"/>
       <c r="J36" s="35"/>
       <c r="K36" s="28"/>
@@ -2533,7 +2539,7 @@
       <c r="E37" s="34"/>
       <c r="F37" s="35"/>
       <c r="G37" s="36"/>
-      <c r="H37" s="89"/>
+      <c r="H37" s="92"/>
       <c r="I37" s="34"/>
       <c r="J37" s="35"/>
       <c r="K37" s="28"/>
@@ -2554,7 +2560,7 @@
       <c r="E38" s="34"/>
       <c r="F38" s="35"/>
       <c r="G38" s="36"/>
-      <c r="H38" s="89"/>
+      <c r="H38" s="92"/>
       <c r="I38" s="34"/>
       <c r="J38" s="35"/>
       <c r="K38" s="28"/>
@@ -2573,7 +2579,7 @@
       <c r="E39" s="34"/>
       <c r="F39" s="35"/>
       <c r="G39" s="36"/>
-      <c r="H39" s="89"/>
+      <c r="H39" s="92"/>
       <c r="I39" s="34"/>
       <c r="J39" s="35"/>
       <c r="K39" s="28"/>
@@ -2592,7 +2598,7 @@
       <c r="E40" s="47"/>
       <c r="F40" s="48"/>
       <c r="G40" s="49"/>
-      <c r="H40" s="90"/>
+      <c r="H40" s="93"/>
       <c r="I40" s="47"/>
       <c r="J40" s="48"/>
       <c r="K40" s="30"/>
@@ -2635,11 +2641,11 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
@@ -2647,11 +2653,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2827,7 +2833,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="98">
+      <c r="A23" s="104">
         <v>45341</v>
       </c>
       <c r="B23" s="78" t="s">
@@ -2838,7 +2844,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="51" t="s">
         <v>84</v>
       </c>
@@ -2847,7 +2853,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="99"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="55" t="s">
         <v>85</v>
       </c>
@@ -2856,7 +2862,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
+      <c r="A26" s="105"/>
       <c r="B26" s="55" t="s">
         <v>86</v>
       </c>
@@ -2865,7 +2871,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="50" t="s">
         <v>87</v>
       </c>
@@ -2874,7 +2880,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="100"/>
+      <c r="A28" s="106"/>
       <c r="B28" s="81" t="s">
         <v>88</v>
       </c>
@@ -2932,7 +2938,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="98">
+      <c r="A34" s="104">
         <v>45348</v>
       </c>
       <c r="B34" s="86" t="s">
@@ -2943,7 +2949,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="99"/>
+      <c r="A35" s="105"/>
       <c r="B35" s="55" t="s">
         <v>94</v>
       </c>
@@ -2952,7 +2958,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="99"/>
+      <c r="A36" s="105"/>
       <c r="B36" s="55" t="s">
         <v>95</v>
       </c>
@@ -2961,7 +2967,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="99"/>
+      <c r="A37" s="105"/>
       <c r="B37" s="55" t="s">
         <v>96</v>
       </c>
@@ -2973,7 +2979,7 @@
       <c r="A38" s="101">
         <v>45349</v>
       </c>
-      <c r="B38" s="105" t="s">
+      <c r="B38" s="89" t="s">
         <v>99</v>
       </c>
       <c r="C38" s="87">
@@ -2982,7 +2988,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="102"/>
-      <c r="B39" s="104" t="s">
+      <c r="B39" s="88" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="72">
@@ -2991,7 +2997,7 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="103"/>
-      <c r="B40" s="106" t="s">
+      <c r="B40" s="90" t="s">
         <v>100</v>
       </c>
       <c r="C40" s="82">
@@ -2999,17 +3005,27 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="52"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="52"/>
+      <c r="A41" s="104">
+        <v>45353</v>
+      </c>
+      <c r="B41" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="106"/>
+      <c r="B42" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="82">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
+      <c r="A43" s="77"/>
       <c r="B43" s="18"/>
       <c r="C43" s="52"/>
     </row>
@@ -3025,7 +3041,7 @@
       <c r="B45" s="12"/>
       <c r="C45" s="54">
         <f>SUM(C8:C44)</f>
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3059,7 +3075,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A1:C1"/>
@@ -3078,26 +3095,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005527F882C56960409CF3FB2B047920CD" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07b97e13f27cbcfe17b734c6cbb54e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fec9890b-0385-4b97-bf60-756cae999a32" xmlns:ns3="0628bb02-9a5c-4726-9a61-75fde915aaf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb78319e54262cd22c56c9b99a05c90" ns2:_="" ns3:_="">
     <xsd:import namespace="fec9890b-0385-4b97-bf60-756cae999a32"/>
@@ -3352,10 +3349,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
+    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3372,20 +3400,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
-    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
JS et PHP doc
</commit_message>
<xml_diff>
--- a/documentation/151 - planning et journal - GENDRE.xlsx
+++ b/documentation/151 - planning et journal - GENDRE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Git\module-151-Gendres\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151-Gendres\git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17BB562-FA29-4244-B16E-DE4BB6E1CF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8ADD96-AA72-49B2-87B5-EAA130503B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="106">
   <si>
     <t>Tâches</t>
   </si>
@@ -441,6 +441,15 @@
   </si>
   <si>
     <t>ajout du mode admin (weekend)</t>
+  </si>
+  <si>
+    <t>correction de bugs et nettoyage du code</t>
+  </si>
+  <si>
+    <t>Tests fonctionnels</t>
+  </si>
+  <si>
+    <t>JS et PHP doc</t>
   </si>
 </sst>
 </file>
@@ -1371,6 +1380,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1380,13 +1395,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1706,11 +1715,11 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A17" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="8" customWidth="1"/>
@@ -2525,7 +2534,9 @@
       <c r="L36" s="34"/>
       <c r="M36" s="35"/>
       <c r="N36" s="36"/>
-      <c r="O36" s="34"/>
+      <c r="O36" s="34" t="s">
+        <v>48</v>
+      </c>
       <c r="P36" s="45"/>
       <c r="Q36" s="36"/>
     </row>
@@ -2567,7 +2578,9 @@
       <c r="L38" s="46"/>
       <c r="M38" s="35"/>
       <c r="N38" s="36"/>
-      <c r="O38" s="46"/>
+      <c r="O38" s="46" t="s">
+        <v>48</v>
+      </c>
       <c r="P38" s="35"/>
       <c r="Q38" s="36"/>
     </row>
@@ -2639,13 +2652,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
@@ -2712,7 +2725,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="101">
+      <c r="A10" s="103">
         <v>45327</v>
       </c>
       <c r="B10" s="63" t="s">
@@ -2723,7 +2736,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="102"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="64" t="s">
         <v>62</v>
       </c>
@@ -2732,7 +2745,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="102"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="64" t="s">
         <v>63</v>
       </c>
@@ -2741,7 +2754,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="64" t="s">
         <v>53</v>
       </c>
@@ -2750,7 +2763,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="102"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="64" t="s">
         <v>74</v>
       </c>
@@ -2759,7 +2772,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="102"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="65" t="s">
         <v>75</v>
       </c>
@@ -2768,7 +2781,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="103"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="65" t="s">
         <v>57</v>
       </c>
@@ -2777,7 +2790,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="101">
+      <c r="A17" s="103">
         <v>45328</v>
       </c>
       <c r="B17" s="73" t="s">
@@ -2788,7 +2801,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="102"/>
+      <c r="A18" s="104"/>
       <c r="B18" s="62" t="s">
         <v>78</v>
       </c>
@@ -2797,7 +2810,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="102"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="74" t="s">
         <v>79</v>
       </c>
@@ -2806,7 +2819,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="102"/>
+      <c r="A20" s="104"/>
       <c r="B20" s="62" t="s">
         <v>80</v>
       </c>
@@ -2815,7 +2828,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="62" t="s">
         <v>81</v>
       </c>
@@ -2824,7 +2837,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="102"/>
+      <c r="A22" s="104"/>
       <c r="B22" s="75" t="s">
         <v>82</v>
       </c>
@@ -2833,7 +2846,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="104">
+      <c r="A23" s="101">
         <v>45341</v>
       </c>
       <c r="B23" s="78" t="s">
@@ -2844,7 +2857,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="105"/>
+      <c r="A24" s="106"/>
       <c r="B24" s="51" t="s">
         <v>84</v>
       </c>
@@ -2853,7 +2866,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="105"/>
+      <c r="A25" s="106"/>
       <c r="B25" s="55" t="s">
         <v>85</v>
       </c>
@@ -2862,7 +2875,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
+      <c r="A26" s="106"/>
       <c r="B26" s="55" t="s">
         <v>86</v>
       </c>
@@ -2871,7 +2884,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="105"/>
+      <c r="A27" s="106"/>
       <c r="B27" s="50" t="s">
         <v>87</v>
       </c>
@@ -2880,7 +2893,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="106"/>
+      <c r="A28" s="102"/>
       <c r="B28" s="81" t="s">
         <v>88</v>
       </c>
@@ -2889,7 +2902,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="101">
+      <c r="A29" s="103">
         <v>45342</v>
       </c>
       <c r="B29" s="83" t="s">
@@ -2900,7 +2913,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="102"/>
+      <c r="A30" s="104"/>
       <c r="B30" s="51" t="s">
         <v>89</v>
       </c>
@@ -2909,7 +2922,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="102"/>
+      <c r="A31" s="104"/>
       <c r="B31" s="55" t="s">
         <v>90</v>
       </c>
@@ -2918,7 +2931,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="103"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="81" t="s">
         <v>91</v>
       </c>
@@ -2938,7 +2951,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="104">
+      <c r="A34" s="101">
         <v>45348</v>
       </c>
       <c r="B34" s="86" t="s">
@@ -2949,7 +2962,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="105"/>
+      <c r="A35" s="106"/>
       <c r="B35" s="55" t="s">
         <v>94</v>
       </c>
@@ -2958,7 +2971,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="105"/>
+      <c r="A36" s="106"/>
       <c r="B36" s="55" t="s">
         <v>95</v>
       </c>
@@ -2967,7 +2980,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="105"/>
+      <c r="A37" s="106"/>
       <c r="B37" s="55" t="s">
         <v>96</v>
       </c>
@@ -2976,7 +2989,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="101">
+      <c r="A38" s="103">
         <v>45349</v>
       </c>
       <c r="B38" s="89" t="s">
@@ -2987,7 +3000,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="102"/>
+      <c r="A39" s="104"/>
       <c r="B39" s="88" t="s">
         <v>79</v>
       </c>
@@ -2996,7 +3009,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="103"/>
+      <c r="A40" s="105"/>
       <c r="B40" s="90" t="s">
         <v>100</v>
       </c>
@@ -3005,7 +3018,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="104">
+      <c r="A41" s="101">
         <v>45353</v>
       </c>
       <c r="B41" s="86" t="s">
@@ -3016,7 +3029,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="106"/>
+      <c r="A42" s="102"/>
       <c r="B42" s="81" t="s">
         <v>101</v>
       </c>
@@ -3025,52 +3038,98 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="77"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="52"/>
+      <c r="A43" s="77">
+        <v>45354</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="52">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="53"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A44" s="77"/>
+      <c r="B44" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="77"/>
+      <c r="B45" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="77"/>
+      <c r="B46" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="77"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="52"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="77"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="52"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="77"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="52"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="56"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="54">
-        <f>SUM(C8:C44)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="15" t="s">
+      <c r="B51" s="12"/>
+      <c r="C51" s="54">
+        <f>SUM(C8:C49)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="17" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="16" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="17" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3095,6 +3154,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005527F882C56960409CF3FB2B047920CD" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07b97e13f27cbcfe17b734c6cbb54e9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fec9890b-0385-4b97-bf60-756cae999a32" xmlns:ns3="0628bb02-9a5c-4726-9a61-75fde915aaf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb78319e54262cd22c56c9b99a05c90" ns2:_="" ns3:_="">
     <xsd:import namespace="fec9890b-0385-4b97-bf60-756cae999a32"/>
@@ -3349,27 +3428,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fec9890b-0385-4b97-bf60-756cae999a32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0628bb02-9a5c-4726-9a61-75fde915aaf9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
+    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DAFA2A-9886-4E5D-A1BA-68C0E131A833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3386,23 +3464,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDAB6660-9544-4877-B428-B71D249521C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fec9890b-0385-4b97-bf60-756cae999a32"/>
-    <ds:schemaRef ds:uri="0628bb02-9a5c-4726-9a61-75fde915aaf9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB721BDB-9F5F-4A98-BDDC-DB34308CB936}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>